<commit_message>
some modi on pic
</commit_message>
<xml_diff>
--- a/LabVIEW/IR_LED-ten_films-without_shelter.xlsx
+++ b/LabVIEW/IR_LED-ten_films-without_shelter.xlsx
@@ -2,26 +2,26 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\Data_git\Data_Analysis\LabVIEW\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\98415\Data_Analysis\LabVIEW\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21576" windowHeight="8052" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="lvtemporary_15997" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
   <si>
     <t>Time - Plot 0</t>
   </si>
@@ -39,9 +39,6 @@
   </si>
   <si>
     <t>ln(I/I0)</t>
-  </si>
-  <si>
-    <t>yi</t>
   </si>
   <si>
     <t>r^2</t>
@@ -85,30 +82,42 @@
   <si>
     <t>STAND</t>
   </si>
+  <si>
+    <t>yi(xi)</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>(yi-yi(xi))^2/sigma^2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>sum</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="18"/>
       <color theme="3"/>
-      <name val="Calibri Light"/>
+      <name val="等线 Light"/>
       <family val="2"/>
       <scheme val="major"/>
     </font>
@@ -116,7 +125,7 @@
       <b/>
       <sz val="15"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -124,7 +133,7 @@
       <b/>
       <sz val="13"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -132,35 +141,35 @@
       <b/>
       <sz val="11"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -168,7 +177,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -176,14 +185,14 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -191,14 +200,14 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -206,7 +215,7 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -214,15 +223,22 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -572,48 +588,48 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="20% - 着色 1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - 着色 2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - 着色 3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - 着色 4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - 着色 5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - 着色 6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - 着色 1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - 着色 2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - 着色 3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - 着色 4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - 着色 5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - 着色 6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - 着色 1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - 着色 2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - 着色 3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - 着色 4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - 着色 5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - 着色 6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="标题" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="标题 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="标题 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="标题 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="标题 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="差" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="好" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="汇总" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="计算" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="检查单元格" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="解释性文本" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="警告文本" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="链接单元格" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="适中" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="输出" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="输入" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="着色 1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="着色 2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="着色 3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="着色 4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="着色 5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -629,9 +645,9 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="zh-CN"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -717,7 +733,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="zh-CN"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -850,7 +866,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-6545-43D0-AD96-27903D2C9E79}"/>
             </c:ext>
@@ -864,11 +880,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="539845576"/>
-        <c:axId val="539846560"/>
+        <c:axId val="413062160"/>
+        <c:axId val="655492000"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="539845576"/>
+        <c:axId val="413062160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -940,7 +956,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="zh-CN"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -978,15 +994,15 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="539846560"/>
+        <c:crossAx val="655492000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="539846560"/>
+        <c:axId val="655492000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1058,7 +1074,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="zh-CN"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1096,10 +1112,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="539845576"/>
+        <c:crossAx val="413062160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1139,7 +1155,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="zh-CN"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1169,7 +1185,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="zh-CN"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2040,10 +2056,10 @@
       <selection activeCell="D6752" sqref="D6752"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -59411,27 +59427,29 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L18"/>
+  <dimension ref="A1:O18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="9.85546875" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" customWidth="1"/>
-    <col min="8" max="8" width="14.5703125" customWidth="1"/>
+    <col min="3" max="3" width="9.88671875" customWidth="1"/>
+    <col min="4" max="4" width="10.5546875" customWidth="1"/>
+    <col min="5" max="5" width="12.109375" customWidth="1"/>
+    <col min="8" max="8" width="14.5546875" customWidth="1"/>
+    <col min="13" max="13" width="22.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>4</v>
       </c>
@@ -59439,19 +59457,22 @@
         <v>5</v>
       </c>
       <c r="D1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K1" t="s">
         <v>5</v>
       </c>
       <c r="L1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="M1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -59475,7 +59496,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -59491,7 +59512,7 @@
         <v>0.186</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F3">
         <f t="array" ref="F3:G7">LINEST(C3:C12,D3:D12,FALSE, TRUE)</f>
@@ -59501,7 +59522,7 @@
         <v>0</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J3">
         <v>0.186</v>
@@ -59513,8 +59534,15 @@
         <f t="shared" si="0"/>
         <v>-8.5290299999999999E-2</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M3">
+        <f>(K3-L3)^2/0.029^2</f>
+        <v>0.35698608436486773</v>
+      </c>
+      <c r="O3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -59530,7 +59558,7 @@
         <v>0.372</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F4">
         <v>7.9418954031464477E-3</v>
@@ -59539,7 +59567,7 @@
         <v>#N/A</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J4">
         <v>0.372</v>
@@ -59551,8 +59579,16 @@
         <f t="shared" si="0"/>
         <v>-0.1705806</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M4">
+        <f t="shared" ref="M4:M12" si="3">(K4-L4)^2/0.029^2</f>
+        <v>0.81975075355811511</v>
+      </c>
+      <c r="O4">
+        <f>SUM(M3:M12)</f>
+        <v>8.9904508542504828</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -59568,7 +59604,7 @@
         <v>0.55800000000000005</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F5">
         <v>0.99730750713078886</v>
@@ -59577,7 +59613,7 @@
         <v>2.8984610722926532E-2</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J5">
         <v>0.55800000000000005</v>
@@ -59589,8 +59625,12 @@
         <f t="shared" si="0"/>
         <v>-0.25587090000000001</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M5">
+        <f t="shared" si="3"/>
+        <v>0.428314551015883</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -59606,7 +59646,7 @@
         <v>0.74399999999999999</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F6">
         <v>3333.6272369803196</v>
@@ -59615,7 +59655,7 @@
         <v>9</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J6">
         <v>0.74399999999999999</v>
@@ -59627,8 +59667,12 @@
         <f t="shared" si="0"/>
         <v>-0.3411612</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M6">
+        <f t="shared" si="3"/>
+        <v>2.2262254787704072</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -59644,7 +59688,7 @@
         <v>0.92999999999999994</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F7">
         <v>2.8006057732367298</v>
@@ -59653,7 +59697,7 @@
         <v>7.5609689288362895E-3</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J7">
         <v>0.92999999999999994</v>
@@ -59665,8 +59709,12 @@
         <f t="shared" si="0"/>
         <v>-0.42645149999999998</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M7">
+        <f t="shared" si="3"/>
+        <v>0.97934130042718015</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -59691,8 +59739,12 @@
         <f t="shared" si="0"/>
         <v>-0.51174180000000002</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M8">
+        <f t="shared" si="3"/>
+        <v>1.0722111283370581</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -59717,8 +59769,12 @@
         <f t="shared" si="0"/>
         <v>-0.59703210000000007</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M9">
+        <f t="shared" si="3"/>
+        <v>0.2944555697563383</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -59743,8 +59799,12 @@
         <f t="shared" si="0"/>
         <v>-0.6823224</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M10">
+        <f t="shared" si="3"/>
+        <v>0.19690214985955773</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -59769,8 +59829,12 @@
         <f t="shared" si="0"/>
         <v>-0.76761270000000004</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M11">
+        <f t="shared" si="3"/>
+        <v>1.1435004259746107</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -59795,8 +59859,12 @@
         <f t="shared" si="0"/>
         <v>-0.85290299999999997</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M12">
+        <f t="shared" si="3"/>
+        <v>1.4727634121864648</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B14">
         <f t="array" ref="B14:C18">LINEST(C2:C12,D2:D12,FALSE,TRUE)</f>
         <v>-0.45854575879216652</v>
@@ -59805,7 +59873,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>7.5343435238291838E-3</v>
       </c>
@@ -59813,7 +59881,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>0.99730750713078908</v>
       </c>
@@ -59838,8 +59906,9 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
@@ -59852,11 +59921,11 @@
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -59864,7 +59933,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E1">
         <f t="shared" ref="E1:E11" si="0">A1-(-0.47922)</f>
@@ -59909,7 +59978,7 @@
         <v>-0.19683722552085425</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E3">
         <f t="shared" si="0"/>
@@ -59946,7 +60015,7 @@
         <v>-0.38443076930275494</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E5">
         <f t="shared" si="0"/>
@@ -60044,7 +60113,7 @@
         <v>0</v>
       </c>
       <c r="B15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -60061,7 +60130,7 @@
         <v>0.372</v>
       </c>
       <c r="B17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -60078,7 +60147,7 @@
         <v>0.74399999999999999</v>
       </c>
       <c r="B19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -60116,6 +60185,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>